<commit_message>
Remove the non_global_files field
Closes #109
</commit_message>
<xml_diff>
--- a/cosmx-proteomics/latest/cosmx-proteomics.xlsx
+++ b/cosmx-proteomics/latest/cosmx-proteomics.xlsx
@@ -230,20 +230,6 @@
     </comment>
     <comment ref="AC1" authorId="1">
       <text>
-        <t>A semicolon separated list of non-shared files to be included in the dataset.
-The path assumes the files are located in the "TOP/non-global/" directory. For
-example, for the file is
-TOP/non-global/lab_processed/images/1-tissue-boundary.geojson the value of this
-field would be "./lab_processed/images/1-tissue-boundary.geojson". After ingest,
-these files will be copied to the appropriate locations within the respective
-dataset directory tree. This field is used for internal HuBMAP processing.
-Examples for GeoMx and PhenoCycler are provided in the File Locations
-documentation:
-https://docs.google.com/document/d/1n2McSs9geA9Eli4QWQaB3c9R3wo5d5U1Xd57DWQfN5Q/edit#heading=h.1u82i4axggee</t>
-      </text>
-    </comment>
-    <comment ref="AD1" authorId="1">
-      <text>
         <t>(Required) The string that serves as the definitive identifier for the metadata
 schema version and is readily interpretable by computers for data validation and
 processing. Example: 22bc762a-5020-419d-b170-24253ed9e8d9</t>
@@ -254,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="435">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -274,6 +260,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000195</t>
   </si>
   <si>
+    <t>Olink</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000441</t>
+  </si>
+  <si>
     <t>SNARE-seq2</t>
   </si>
   <si>
@@ -310,6 +302,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
   </si>
   <si>
+    <t>FACS</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000440</t>
+  </si>
+  <si>
     <t>Xenium</t>
   </si>
   <si>
@@ -319,7 +317,7 @@
     <t>Stereo-seq</t>
   </si>
   <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000434</t>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
   </si>
   <si>
     <t>Visium (with probes)</t>
@@ -346,6 +344,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
   </si>
   <si>
+    <t>Seq-Scope</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000390</t>
+  </si>
+  <si>
     <t>SIMS</t>
   </si>
   <si>
@@ -472,6 +476,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000312</t>
   </si>
   <si>
+    <t>Pixel-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000449</t>
+  </si>
+  <si>
     <t>10X Multiome</t>
   </si>
   <si>
@@ -490,6 +500,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000311</t>
   </si>
   <si>
+    <t>4i</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000447</t>
+  </si>
+  <si>
     <t>PhenoCycler</t>
   </si>
   <si>
@@ -520,6 +536,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
   </si>
   <si>
+    <t>MPLEx</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000448</t>
+  </si>
+  <si>
     <t>analyte_class</t>
   </si>
   <si>
@@ -661,6 +683,12 @@
     <t>https://identifiers.org/RRID:SCR_027007</t>
   </si>
   <si>
+    <t>3DHISTECH</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027042</t>
+  </si>
+  <si>
     <t>GE Healthcare</t>
   </si>
   <si>
@@ -775,12 +803,24 @@
     <t>https://identifiers.org/RRID:SCR_023603</t>
   </si>
   <si>
+    <t>Cytek Biosciences</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027071</t>
+  </si>
+  <si>
     <t>10x Genomics</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_023672</t>
   </si>
   <si>
+    <t>Microscopes International</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027094</t>
+  </si>
+  <si>
     <t>Hamamatsu</t>
   </si>
   <si>
@@ -814,6 +854,12 @@
     <t>https://identifiers.org/RRID:SCR_017202</t>
   </si>
   <si>
+    <t>Pannoramic MIDI II Digital Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024834</t>
+  </si>
+  <si>
     <t>Not applicable</t>
   </si>
   <si>
@@ -922,6 +968,12 @@
     <t>https://identifiers.org/RRID:SCR_019916</t>
   </si>
   <si>
+    <t>uScopeHXII-20</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027101</t>
+  </si>
+  <si>
     <t>Custom: Multiphoton</t>
   </si>
   <si>
@@ -1000,6 +1052,12 @@
     <t>https://identifiers.org/RRID:SCR_016381</t>
   </si>
   <si>
+    <t>Axio Zoom.V16</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027090</t>
+  </si>
+  <si>
     <t>Digital Spatial Profiler</t>
   </si>
   <si>
@@ -1036,6 +1094,12 @@
     <t>https://identifiers.org/RRID:SCR_023694</t>
   </si>
   <si>
+    <t>Cytek Northern Lights</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027072</t>
+  </si>
+  <si>
     <t>IN Cell Analyzer 2200</t>
   </si>
   <si>
@@ -1150,6 +1214,12 @@
     <t>https://identifiers.org/RRID:SCR_016386</t>
   </si>
   <si>
+    <t>solariX</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027095</t>
+  </si>
+  <si>
     <t>Aperio AT2</t>
   </si>
   <si>
@@ -1162,6 +1232,12 @@
     <t>https://identifiers.org/RRID:SCR_023613</t>
   </si>
   <si>
+    <t>Biomark HD</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_022658</t>
+  </si>
+  <si>
     <t>NanoZoomer S60</t>
   </si>
   <si>
@@ -1186,6 +1262,12 @@
     <t>https://identifiers.org/RRID:SCR_020927</t>
   </si>
   <si>
+    <t>Juno System</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027198</t>
+  </si>
+  <si>
     <t>Q Exactive HF</t>
   </si>
   <si>
@@ -1309,6 +1391,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000383</t>
   </si>
   <si>
+    <t>10x Genomics; Xenium Mouse Multi-Tissue Atlassing Panel; PN 1000627</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000442</t>
+  </si>
+  <si>
     <t>10x Genomics; Visium Human Transcriptome Probe Kit-Small; PN 1000363</t>
   </si>
   <si>
@@ -1351,12 +1439,30 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000395</t>
   </si>
   <si>
+    <t>10x Genomics; Xenium Custom Gene Expression Panel (up to 50 genes); PN 1000464</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000445</t>
+  </si>
+  <si>
+    <t>10x Genomics; Xenium Custom Gene Expression Panel (51-100 genes); PN 1000561</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000444</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Human Transcriptome Probe Kit, 64 rxns; PN 1000456</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000376</t>
   </si>
   <si>
+    <t>10x Genomics; Xenium Human Colon Gene Expression Panel; PN 1000642</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000446</t>
+  </si>
+  <si>
     <t>NanoString Technologies; CosMx Human Immuno-Oncology Panel (Protein, 64 Plex); PN CMX-H-IOP-64P-P</t>
   </si>
   <si>
@@ -1375,6 +1481,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000362</t>
   </si>
   <si>
+    <t>10x Genomics; Xenium Human Lung Gene Expression Panel; PN 1000601</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000443</t>
+  </si>
+  <si>
     <t>NanoString Technologies; CosMx Human Universal Cell Characterization Panel (RNA, 1000 Plex); PN CMX-H-USCP-1KP-R</t>
   </si>
   <si>
@@ -1408,9 +1520,6 @@
     <t>anatomical_structure_id</t>
   </si>
   <si>
-    <t>non_global_files</t>
-  </si>
-  <si>
     <t>metadata_schema_id</t>
   </si>
   <si>
@@ -1429,7 +1538,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-06-06T07:54:49-07:00</t>
+    <t>2025-07-24T21:05:52-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1488,7 +1597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyAlignment="true" applyFill="true">
       <alignment horizontal="center"/>
@@ -1522,7 +1631,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -1533,7 +1641,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AD2"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1567,8 +1675,7 @@
     <col min="26" max="26" style="27" width="7.4296875" customWidth="true" bestFit="true"/>
     <col min="27" max="27" style="28" width="21.44921875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" style="29" width="19.23828125" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" style="30" width="13.33984375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" style="31" width="16.91796875" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" style="30" width="16.91796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1585,96 +1692,93 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>314</v>
+        <v>346</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>315</v>
+        <v>347</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>326</v>
+        <v>358</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>327</v>
+        <v>359</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>328</v>
+        <v>360</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>329</v>
+        <v>361</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>330</v>
+        <v>362</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>331</v>
+        <v>363</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>336</v>
+        <v>368</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>337</v>
+        <v>369</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>338</v>
+        <v>370</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>339</v>
+        <v>371</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>340</v>
+        <v>372</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>341</v>
+        <v>373</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>342</v>
+        <v>374</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>379</v>
+        <v>421</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>380</v>
+        <v>422</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>381</v>
+        <v>423</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>382</v>
+        <v>424</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>383</v>
+        <v>425</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>384</v>
-      </c>
-      <c r="AD1" t="s" s="1">
-        <v>385</v>
+        <v>426</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>52</v>
-      </c>
-      <c r="AD2" t="s" s="31">
-        <v>386</v>
+        <v>58</v>
+      </c>
+      <c r="AC2" t="s" s="30">
+        <v>427</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="19">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$42</formula1>
+      <formula1>'dataset_type'!$A$1:$A$48</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -1683,10 +1787,10 @@
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$27</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$30</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$68</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$75</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1728,7 +1832,7 @@
       <formula1>'probe_hybridization_time_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="W2:W1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'oligo_probe_panel'!$A$1:$A$18</formula1>
+      <formula1>'oligo_probe_panel'!$A$1:$A$23</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="X2:X1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_custom_probes_used'!$A$1:$A$2</formula1>
@@ -1754,10 +1858,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>324</v>
+        <v>356</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>325</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -1775,18 +1879,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>316</v>
+        <v>348</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>317</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>324</v>
+        <v>356</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>325</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -1796,7 +1900,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1804,146 +1908,186 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>343</v>
+        <v>375</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>344</v>
+        <v>376</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>345</v>
+        <v>377</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>346</v>
+        <v>378</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>347</v>
+        <v>379</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>348</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>349</v>
+        <v>381</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>350</v>
+        <v>382</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>351</v>
+        <v>383</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>352</v>
+        <v>384</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>353</v>
+        <v>385</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>354</v>
+        <v>386</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>355</v>
+        <v>387</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>356</v>
+        <v>388</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>357</v>
+        <v>389</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>358</v>
+        <v>390</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>359</v>
+        <v>391</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>360</v>
+        <v>392</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>361</v>
+        <v>393</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>362</v>
+        <v>394</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>363</v>
+        <v>395</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>364</v>
+        <v>396</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>365</v>
+        <v>397</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>366</v>
+        <v>398</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>367</v>
+        <v>399</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>368</v>
+        <v>400</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>369</v>
+        <v>401</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>370</v>
+        <v>402</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>371</v>
+        <v>403</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>372</v>
+        <v>404</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>373</v>
+        <v>405</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>374</v>
+        <v>406</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>375</v>
+        <v>407</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>376</v>
+        <v>408</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>377</v>
+        <v>409</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>378</v>
+        <v>410</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>411</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>413</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>415</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>417</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>419</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>420</v>
       </c>
     </row>
   </sheetData>
@@ -1961,12 +2105,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>122</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>123</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1990,30 +2134,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>387</v>
+        <v>428</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>388</v>
+        <v>429</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>390</v>
+        <v>431</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>392</v>
+        <v>433</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>389</v>
+        <v>430</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>391</v>
+        <v>432</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>393</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -2023,7 +2167,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2363,6 +2507,54 @@
       </c>
       <c r="B42" t="s" s="0">
         <v>87</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2380,130 +2572,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>90</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>92</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>94</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>96</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>98</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>100</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>102</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>104</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>106</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>108</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>110</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>112</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>114</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>116</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>118</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>120</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2521,12 +2713,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>122</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>123</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2536,7 +2728,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2544,218 +2736,242 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>126</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>128</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>130</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>132</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>134</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>136</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>138</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>140</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>142</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>144</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>146</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>148</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>150</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>152</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>154</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>156</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>158</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>160</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>162</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>164</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>166</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>168</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>170</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>172</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>174</v>
+        <v>186</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>176</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>178</v>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>191</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>193</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>195</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -2765,7 +2981,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B68"/>
+  <dimension ref="A1:B75"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2773,546 +2989,602 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>181</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>182</v>
+        <v>200</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>183</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>185</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>186</v>
+        <v>204</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>187</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>189</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>191</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>193</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>194</v>
+        <v>212</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>195</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>196</v>
+        <v>214</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>197</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>198</v>
+        <v>216</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>199</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>200</v>
+        <v>218</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>201</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>203</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>205</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>206</v>
+        <v>224</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>207</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>209</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>211</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>213</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>214</v>
+        <v>232</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>215</v>
+        <v>233</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>216</v>
+        <v>234</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>217</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>218</v>
+        <v>236</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>219</v>
+        <v>237</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>220</v>
+        <v>238</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>221</v>
+        <v>239</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>222</v>
+        <v>240</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>223</v>
+        <v>241</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>224</v>
+        <v>242</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>225</v>
+        <v>243</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>226</v>
+        <v>244</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>227</v>
+        <v>245</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>228</v>
+        <v>246</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>229</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>231</v>
+        <v>249</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>232</v>
+        <v>250</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>233</v>
+        <v>251</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>234</v>
+        <v>252</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>235</v>
+        <v>253</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>237</v>
+        <v>255</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>238</v>
+        <v>256</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>239</v>
+        <v>257</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>240</v>
+        <v>258</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>241</v>
+        <v>259</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>242</v>
+        <v>260</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>243</v>
+        <v>261</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>244</v>
+        <v>262</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>245</v>
+        <v>263</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>246</v>
+        <v>264</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>247</v>
+        <v>265</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>248</v>
+        <v>266</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>249</v>
+        <v>267</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>250</v>
+        <v>268</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>251</v>
+        <v>269</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>252</v>
+        <v>270</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>253</v>
+        <v>271</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>254</v>
+        <v>272</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>255</v>
+        <v>273</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>256</v>
+        <v>274</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>257</v>
+        <v>275</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>258</v>
+        <v>276</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>259</v>
+        <v>277</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>260</v>
+        <v>278</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>261</v>
+        <v>279</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>262</v>
+        <v>280</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>263</v>
+        <v>281</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>264</v>
+        <v>282</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>265</v>
+        <v>283</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>266</v>
+        <v>284</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>267</v>
+        <v>285</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>268</v>
+        <v>286</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>269</v>
+        <v>287</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>270</v>
+        <v>288</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>271</v>
+        <v>289</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>272</v>
+        <v>290</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>273</v>
+        <v>291</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>274</v>
+        <v>292</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>275</v>
+        <v>293</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>276</v>
+        <v>294</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>277</v>
+        <v>295</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>278</v>
+        <v>296</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>279</v>
+        <v>297</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>280</v>
+        <v>298</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>281</v>
+        <v>299</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>282</v>
+        <v>300</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>283</v>
+        <v>301</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>284</v>
+        <v>302</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>285</v>
+        <v>303</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>286</v>
+        <v>304</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>287</v>
+        <v>305</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>288</v>
+        <v>306</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>289</v>
+        <v>307</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>290</v>
+        <v>308</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>291</v>
+        <v>309</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>292</v>
+        <v>310</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>293</v>
+        <v>311</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>294</v>
+        <v>312</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>295</v>
+        <v>313</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>153</v>
+        <v>314</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>154</v>
+        <v>315</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>296</v>
+        <v>316</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>297</v>
+        <v>317</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>298</v>
+        <v>318</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>299</v>
+        <v>319</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>301</v>
+        <v>321</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>302</v>
+        <v>167</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>303</v>
+        <v>168</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>304</v>
+        <v>322</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>305</v>
+        <v>323</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>306</v>
+        <v>324</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>307</v>
+        <v>325</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>308</v>
+        <v>326</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>309</v>
+        <v>327</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>310</v>
+        <v>328</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>311</v>
+        <v>329</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>312</v>
+        <v>330</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>313</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="0">
+        <v>332</v>
+      </c>
+      <c r="B69" t="s" s="0">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="0">
+        <v>334</v>
+      </c>
+      <c r="B70" t="s" s="0">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="0">
+        <v>336</v>
+      </c>
+      <c r="B71" t="s" s="0">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="0">
+        <v>338</v>
+      </c>
+      <c r="B72" t="s" s="0">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="0">
+        <v>340</v>
+      </c>
+      <c r="B73" t="s" s="0">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="0">
+        <v>342</v>
+      </c>
+      <c r="B74" t="s" s="0">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="0">
+        <v>344</v>
+      </c>
+      <c r="B75" t="s" s="0">
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -3330,42 +3602,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>316</v>
+        <v>348</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>317</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>318</v>
+        <v>350</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>319</v>
+        <v>351</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>320</v>
+        <v>352</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>321</v>
+        <v>353</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>322</v>
+        <v>354</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>323</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>324</v>
+        <v>356</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>325</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -3383,26 +3655,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>318</v>
+        <v>350</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>319</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>320</v>
+        <v>352</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>321</v>
+        <v>353</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>322</v>
+        <v>354</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>323</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -3420,18 +3692,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>332</v>
+        <v>364</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>333</v>
+        <v>365</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>334</v>
+        <v>366</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>335</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new oligo probe panels
Closes #117
</commit_message>
<xml_diff>
--- a/cosmx-proteomics/latest/cosmx-proteomics.xlsx
+++ b/cosmx-proteomics/latest/cosmx-proteomics.xlsx
@@ -240,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="446">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -260,48 +260,168 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000195</t>
   </si>
   <si>
+    <t>SNARE-seq2</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000264</t>
+  </si>
+  <si>
+    <t>Visium (no probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
+  </si>
+  <si>
+    <t>DESI</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
+  </si>
+  <si>
+    <t>Confocal</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
+  </si>
+  <si>
+    <t>Stereo-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
+  </si>
+  <si>
+    <t>Visium (with probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
+  </si>
+  <si>
+    <t>Molecular Cartography</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
+  </si>
+  <si>
+    <t>CosMx</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
+  </si>
+  <si>
+    <t>DBiT-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
+  </si>
+  <si>
+    <t>Seq-Scope</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000390</t>
+  </si>
+  <si>
+    <t>CyCIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
+  </si>
+  <si>
+    <t>Light Sheet</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+  </si>
+  <si>
+    <t>seqFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
+  </si>
+  <si>
+    <t>ATACseq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
+  </si>
+  <si>
+    <t>CosMx Proteomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
+  </si>
+  <si>
+    <t>Singular Genomics G4X</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
+  </si>
+  <si>
+    <t>Visium HD</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000451</t>
+  </si>
+  <si>
+    <t>MERFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
+  </si>
+  <si>
+    <t>10X Multiome</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
+  </si>
+  <si>
+    <t>4i</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000447</t>
+  </si>
+  <si>
+    <t>PhenoCycler</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
+  </si>
+  <si>
+    <t>Second Harmonic Generation (SHG)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
+  </si>
+  <si>
+    <t>Thick section Multiphoton MxIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
+  </si>
+  <si>
+    <t>CyTOF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
+  </si>
+  <si>
     <t>Olink</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000441</t>
   </si>
   <si>
-    <t>SNARE-seq2</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000264</t>
-  </si>
-  <si>
     <t>MIBI</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000172</t>
   </si>
   <si>
-    <t>Visium (no probes)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
-  </si>
-  <si>
-    <t>DESI</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
-  </si>
-  <si>
     <t>Auto-fluorescence</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000205</t>
   </si>
   <si>
-    <t>Confocal</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
-  </si>
-  <si>
     <t>FACS</t>
   </si>
   <si>
@@ -314,42 +434,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000219</t>
   </si>
   <si>
-    <t>Stereo-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
-  </si>
-  <si>
-    <t>Visium (with probes)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
-  </si>
-  <si>
-    <t>Molecular Cartography</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
-  </si>
-  <si>
-    <t>CosMx</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
-  </si>
-  <si>
-    <t>DBiT-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
-  </si>
-  <si>
-    <t>Seq-Scope</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000390</t>
-  </si>
-  <si>
     <t>SIMS</t>
   </si>
   <si>
@@ -380,16 +464,10 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000328</t>
   </si>
   <si>
-    <t>CyCIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
-  </si>
-  <si>
-    <t>Light Sheet</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+    <t>Pixel-seqV2</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000450</t>
   </si>
   <si>
     <t>MALDI</t>
@@ -398,30 +476,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000201</t>
   </si>
   <si>
-    <t>seqFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
-  </si>
-  <si>
     <t>2D Imaging Mass Cytometry</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000296</t>
   </si>
   <si>
-    <t>ATACseq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
-  </si>
-  <si>
-    <t>CosMx Proteomics</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
-  </si>
-  <si>
     <t>Histology</t>
   </si>
   <si>
@@ -452,18 +512,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000310</t>
   </si>
   <si>
-    <t>Singular Genomics G4X</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
-  </si>
-  <si>
-    <t>MERFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
-  </si>
-  <si>
     <t>LC-MS</t>
   </si>
   <si>
@@ -476,18 +524,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000312</t>
   </si>
   <si>
-    <t>Pixel-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000449</t>
-  </si>
-  <si>
-    <t>10X Multiome</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
-  </si>
-  <si>
     <t>GeoMx (nCounter)</t>
   </si>
   <si>
@@ -500,42 +536,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000311</t>
   </si>
   <si>
-    <t>4i</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000447</t>
-  </si>
-  <si>
-    <t>PhenoCycler</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
-  </si>
-  <si>
-    <t>Second Harmonic Generation (SHG)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
-  </si>
-  <si>
-    <t>Thick section Multiphoton MxIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
-  </si>
-  <si>
     <t>MS Lipidomics</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000405</t>
   </si>
   <si>
-    <t>CyTOF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
-  </si>
-  <si>
     <t>MPLEx</t>
   </si>
   <si>
@@ -1190,6 +1196,9 @@
     <t>https://identifiers.org/RRID:SCR_023618</t>
   </si>
   <si>
+    <t>https://identifiers.org/RRID:SCR_027323</t>
+  </si>
+  <si>
     <t>MERSCOPE</t>
   </si>
   <si>
@@ -1367,46 +1376,118 @@
     <t>oligo_probe_panel</t>
   </si>
   <si>
+    <t>10x Genomics; Chromium Next GEM Single Cell Fixed RNA Mouse Transcriptome Probe Kit, 64 rxns; PN 1000492</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000393</t>
+  </si>
+  <si>
+    <t>10x Genomics; Xenium Prime 5K Human Pan Tissue &amp; Pathways Panel; PN 1000724</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000426</t>
+  </si>
+  <si>
+    <t>10x Genomics; Visium Human Transcriptome Probe Kit-Large; PN 1000364</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000383</t>
+  </si>
+  <si>
+    <t>10x Genomics; Xenium Mouse Multi-Tissue Atlassing Panel; PN 1000627</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000442</t>
+  </si>
+  <si>
+    <t>10x Genomics; Visium Human Transcriptome Probe Kit-Small; PN 1000363</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000326</t>
+  </si>
+  <si>
+    <t>10x Genomics; Visium Mouse Transcriptome Probe Kit v2.0 - Small; PN 1000667</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000431</t>
+  </si>
+  <si>
+    <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome 4 rxns x 4 BC; PN 1000475</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000307</t>
+  </si>
+  <si>
+    <t>10x Genomics; Visium Human Transcriptome Probe Kit v2 - Small; PN 1000466</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000274</t>
+  </si>
+  <si>
+    <t>NanoString Technologies; CosMx Human 6K Discovery Panel (RNA, 6175 Plex); PN 121500041</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000455</t>
+  </si>
+  <si>
+    <t>10x Genomics; Xenium Custom Gene Expression Panel (51-100 genes); PN 1000561</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000444</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Human Transcriptome Probe Kit, 64 rxns; PN 1000456</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000376</t>
+  </si>
+  <si>
+    <t>10x Genomics; Xenium Human Colon Gene Expression Panel; PN 1000642</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000446</t>
+  </si>
+  <si>
+    <t>NanoString Technologies; CosMx Human Immuno-Oncology Panel (Protein, 64 Plex); PN CMX-H-IOP-64P-P</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000436</t>
+  </si>
+  <si>
+    <t>10x Genomics; Visium Mouse Transcriptome Probe Kit - Small; PN 1000365</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000362</t>
+  </si>
+  <si>
+    <t>NanoString Technologies; CosMx Hs WTX RNA Panel Kit, 2 slides: PN 121500047</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000453</t>
+  </si>
+  <si>
+    <t>10x Genomics; Xenium Human Lung Gene Expression Panel; PN 1000601</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000443</t>
+  </si>
+  <si>
+    <t>NanoString Technologies; CosMx Mouse Neuroscience Panel (Protein, 64 Plex); PN CMX-M-Neuro-64P-P</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000437</t>
+  </si>
+  <si>
     <t>NanoString Technologies; GeoMx Mouse Whole Transcriptome Atlas, 4 slides; PN GMX-RNA-NGS-MsWTA-4</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000364</t>
   </si>
   <si>
-    <t>10x Genomics; Chromium Next GEM Single Cell Fixed RNA Mouse Transcriptome Probe Kit, 64 rxns; PN 1000492</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000393</t>
-  </si>
-  <si>
-    <t>10x Genomics; Xenium Prime 5K Human Pan Tissue &amp; Pathways Panel; PN 1000724</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000426</t>
-  </si>
-  <si>
-    <t>10x Genomics; Visium Human Transcriptome Probe Kit-Large; PN 1000364</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000383</t>
-  </si>
-  <si>
-    <t>10x Genomics; Xenium Mouse Multi-Tissue Atlassing Panel; PN 1000627</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000442</t>
-  </si>
-  <si>
-    <t>10x Genomics; Visium Human Transcriptome Probe Kit-Small; PN 1000363</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000326</t>
-  </si>
-  <si>
-    <t>10x Genomics; Visium Mouse Transcriptome Probe Kit v2.0 - Small; PN 1000667</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000431</t>
+    <t>NanoString Technologies; CosMx Mouse Neuroscience Panel (RNA, 1000 Plex); PN CMX-M-NEUP-R</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000452</t>
   </si>
   <si>
     <t>Custom</t>
@@ -1421,18 +1502,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000363</t>
   </si>
   <si>
-    <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome 4 rxns x 4 BC; PN 1000475</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000307</t>
-  </si>
-  <si>
-    <t>10x Genomics; Visium Human Transcriptome Probe Kit v2 - Small; PN 1000466</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000274</t>
-  </si>
-  <si>
     <t>10x Genomics; Xenium Human Multi-Tissue and Cancer Panel v1; PN 1000626</t>
   </si>
   <si>
@@ -1445,66 +1514,30 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000445</t>
   </si>
   <si>
-    <t>10x Genomics; Xenium Custom Gene Expression Panel (51-100 genes); PN 1000561</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000444</t>
-  </si>
-  <si>
-    <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Human Transcriptome Probe Kit, 64 rxns; PN 1000456</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000376</t>
-  </si>
-  <si>
-    <t>10x Genomics; Xenium Human Colon Gene Expression Panel; PN 1000642</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000446</t>
-  </si>
-  <si>
-    <t>NanoString Technologies; CosMx Human Immuno-Oncology Panel (Protein, 64 Plex); PN CMX-H-IOP-64P-P</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000436</t>
-  </si>
-  <si>
     <t>10x Genomics; Chromium Fixed RNA Kit, Human Transcriptome, 4 rxns x 1 BC; PN 1000474</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000306</t>
   </si>
   <si>
-    <t>10x Genomics; Visium Mouse Transcriptome Probe Kit - Small; PN 1000365</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000362</t>
-  </si>
-  <si>
-    <t>10x Genomics; Xenium Human Lung Gene Expression Panel; PN 1000601</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000443</t>
-  </si>
-  <si>
     <t>NanoString Technologies; CosMx Human Universal Cell Characterization Panel (RNA, 1000 Plex); PN CMX-H-USCP-1KP-R</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000430</t>
   </si>
   <si>
-    <t>NanoString Technologies; CosMx Mouse Neuroscience Panel (Protein, 64 Plex); PN CMX-M-Neuro-64P-P</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000437</t>
-  </si>
-  <si>
     <t>10X Genomics; Chromium Next GEM Single Cell Fixed RNA Human Transcriptome Probe Kit, 16 rxns; PN 1000420</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000382</t>
   </si>
   <si>
+    <t>NanoString Technologies; CosMx Hs Univ Cell (RNA, 1000 Plex); PN 121500002</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000454</t>
+  </si>
+  <si>
     <t>is_custom_probes_used</t>
   </si>
   <si>
@@ -1538,7 +1571,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-07-24T21:05:52-07:00</t>
+    <t>2025-09-11T14:00:48-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1692,93 +1725,93 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>421</v>
+        <v>432</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>422</v>
+        <v>433</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>423</v>
+        <v>434</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>424</v>
+        <v>435</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>425</v>
+        <v>436</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>426</v>
+        <v>437</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="AC2" t="s" s="30">
-        <v>427</v>
+        <v>438</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="19">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$48</formula1>
+      <formula1>'dataset_type'!$A$1:$A$49</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -1790,7 +1823,7 @@
       <formula1>'acquisition_instrument_vendor'!$A$1:$A$30</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$75</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$76</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1832,7 +1865,7 @@
       <formula1>'probe_hybridization_time_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="W2:W1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'oligo_probe_panel'!$A$1:$A$23</formula1>
+      <formula1>'oligo_probe_panel'!$A$1:$A$27</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="X2:X1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_custom_probes_used'!$A$1:$A$2</formula1>
@@ -1858,10 +1891,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -1879,18 +1912,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -1900,7 +1933,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1908,186 +1941,218 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>378</v>
+        <v>381</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>382</v>
+        <v>385</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>384</v>
+        <v>387</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>386</v>
+        <v>389</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>390</v>
+        <v>393</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>392</v>
+        <v>395</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>394</v>
+        <v>397</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>398</v>
+        <v>401</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>400</v>
+        <v>403</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>402</v>
+        <v>405</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>404</v>
+        <v>407</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>406</v>
+        <v>409</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>408</v>
+        <v>411</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>412</v>
+        <v>415</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>414</v>
+        <v>417</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>416</v>
+        <v>419</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>418</v>
+        <v>421</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>420</v>
+        <v>423</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>424</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>426</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>428</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>430</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -2105,12 +2170,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2134,30 +2199,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>428</v>
+        <v>439</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>429</v>
+        <v>440</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>431</v>
+        <v>442</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>433</v>
+        <v>444</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>430</v>
+        <v>441</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>432</v>
+        <v>443</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>434</v>
+        <v>445</v>
       </c>
     </row>
   </sheetData>
@@ -2167,7 +2232,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2555,6 +2620,14 @@
       </c>
       <c r="B48" t="s" s="0">
         <v>99</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2572,130 +2645,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2713,12 +2786,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2736,242 +2809,242 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2981,7 +3054,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B75"/>
+  <dimension ref="A1:B76"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2989,602 +3062,610 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>316</v>
+        <v>66</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>167</v>
+        <v>323</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>168</v>
+        <v>324</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>322</v>
+        <v>169</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>323</v>
+        <v>170</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="0">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="0">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="0">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="0">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s" s="0">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B74" t="s" s="0">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s" s="0">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B75" t="s" s="0">
-        <v>345</v>
+        <v>346</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="0">
+        <v>347</v>
+      </c>
+      <c r="B76" t="s" s="0">
+        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -3602,42 +3683,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>355</v>
+        <v>358</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -3655,26 +3736,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>355</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -3692,18 +3773,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>367</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new non_global_files field
Closes #118
</commit_message>
<xml_diff>
--- a/cosmx-proteomics/latest/cosmx-proteomics.xlsx
+++ b/cosmx-proteomics/latest/cosmx-proteomics.xlsx
@@ -230,6 +230,20 @@
     </comment>
     <comment ref="AC1" authorId="1">
       <text>
+        <t>A semicolon separated list of non-shared files to be included in the dataset.
+The path assumes the files are located in the "TOP/non-global/" directory. For
+example, for the file is
+TOP/non-global/lab_processed/images/1-tissue-boundary.geojson the value of this
+field would be "./lab_processed/images/1-tissue-boundary.geojson". After ingest,
+these files will be copied to the appropriate locations within the respective
+dataset directory tree. This field is used for internal HuBMAP processing.
+Examples for GeoMx and PhenoCycler are provided in the File Locations
+documentation:
+https://docs.google.com/document/d/1n2McSs9geA9Eli4QWQaB3c9R3wo5d5U1Xd57DWQfN5Q/edit#heading=h.1u82i4axggee</t>
+      </text>
+    </comment>
+    <comment ref="AD1" authorId="1">
+      <text>
         <t>(Required) The string that serves as the definitive identifier for the metadata
 schema version and is readily interpretable by computers for data validation and
 processing. Example: 22bc762a-5020-419d-b170-24253ed9e8d9</t>
@@ -240,7 +254,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="447">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -302,24 +316,24 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
   </si>
   <si>
-    <t>CosMx</t>
+    <t>DBiT-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
+  </si>
+  <si>
+    <t>Seq-Scope</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000390</t>
+  </si>
+  <si>
+    <t>CosMx Transcriptomics</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
   </si>
   <si>
-    <t>DBiT-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
-  </si>
-  <si>
-    <t>Seq-Scope</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000390</t>
-  </si>
-  <si>
     <t>CyCIF</t>
   </si>
   <si>
@@ -1553,6 +1567,9 @@
     <t>anatomical_structure_id</t>
   </si>
   <si>
+    <t>non_global_files</t>
+  </si>
+  <si>
     <t>metadata_schema_id</t>
   </si>
   <si>
@@ -1571,7 +1588,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-09-15T07:59:29-07:00</t>
+    <t>2025-09-18T09:02:19-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1630,7 +1647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyAlignment="true" applyFill="true">
       <alignment horizontal="center"/>
@@ -1664,6 +1681,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -1674,7 +1692,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1708,7 +1726,8 @@
     <col min="26" max="26" style="27" width="7.4296875" customWidth="true" bestFit="true"/>
     <col min="27" max="27" style="28" width="21.44921875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" style="29" width="19.23828125" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" style="30" width="16.91796875" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" style="30" width="13.33984375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" style="31" width="16.91796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1799,13 +1818,16 @@
       <c r="AC1" t="s" s="1">
         <v>437</v>
       </c>
+      <c r="AD1" t="s" s="1">
+        <v>438</v>
+      </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
         <v>34</v>
       </c>
-      <c r="AC2" t="s" s="30">
-        <v>438</v>
+      <c r="AD2" t="s" s="31">
+        <v>439</v>
       </c>
     </row>
   </sheetData>
@@ -2199,16 +2221,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="2">
@@ -2216,13 +2238,13 @@
         <v>34</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update CosMx new oligo panel
Closes #122
</commit_message>
<xml_diff>
--- a/cosmx-proteomics/latest/cosmx-proteomics.xlsx
+++ b/cosmx-proteomics/latest/cosmx-proteomics.xlsx
@@ -33,219 +33,235 @@
   <commentList>
     <comment ref="A1" authorId="1">
       <text>
-        <t>(Required) Unique HuBMAP or SenNet identifier of the sample (i.e., block,
-section or suspension) used to perform this assay. For example, for a RNAseq
-assay, the parent would be the suspension, whereas, for one of the imaging
-assays, the parent would be the tissue section. If an assay comes from multiple
-parent samples then this should be a comma separated list. Example:
-HBM386.ZGKG.235, HBM672.MKPK.442 or SNT232.UBHJ.322, SNT329.ALSK.102</t>
+        <t>(Required) The unique identifier from HuBMAP or SenNet for the sample (such as a
+block, section, or suspension) used to perform the assay. For instance, in an
+RNAseq assay, the parent sample would be the suspension, while in imaging
+assays, it would be the tissue section. If the assay is derived from multiple
+parent samples, this field should contain a comma-separated list of identifiers.
+Example: HBM386.ZGKG.235, HBM672.MKPK.442</t>
       </text>
     </comment>
     <comment ref="B1" authorId="1">
       <text>
-        <t>An internal field labs can use it to add whatever ID(s) they want or need for
-dataset validation and tracking. This could be a single ID (e.g.,
-"Visium_9OLC_A4_S1") or a delimited list of IDs (e.g., “9OL; 9OLC.A2;
-Visium_9OLC_A4_S1”). This field will not be accessible to anyone outside of the
-consortium and no effort will be made to check if IDs provided by one data
-provider are also used by another.</t>
+        <t>A locally assigned identifier provided by the data provider for the dataset. It
+is used to reference an external metadata record that may be maintained
+independently, enabling traceability and supporting provenance tracking.
+Example: Visium_9OLC_A4_S1</t>
       </text>
     </comment>
     <comment ref="C1" authorId="1">
       <text>
-        <t>(Required) DOI for the protocols.io page that describes the assay or sample
-procurement and preparation. For example for an imaging assay, the protocol
-might begin with staining of a section and finalize with the creation of an
-OME-TIFF file. In this case the protocol would include any image processing
-steps required to create the OME-TIFF file. Example:
-https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1.</t>
+        <t>The DOI for the protocols.io page that details the assay or the procedures used
+for sample procurement and preparation. For example, in the case of an imaging
+assay, the protocol may start with tissue section staining and end with the
+generation of an OME-TIFF file. The documented protocol should also include any
+image processing steps involved in producing the final OME-TIFF. Example:
+https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1</t>
       </text>
     </comment>
     <comment ref="D1" authorId="1">
       <text>
-        <t>(Required) The specific type of dataset being produced.</t>
+        <t>(Required) The specific type of dataset being produced. Example: RNAseq</t>
       </text>
     </comment>
     <comment ref="E1" authorId="1">
       <text>
-        <t>(Required) Analytes are the target molecules being measured with the assay.</t>
+        <t>(Required) The analyte class which is the target molecule that the assay is
+measuring. Example: DNA</t>
       </text>
     </comment>
     <comment ref="F1" authorId="1">
       <text>
-        <t>(Required) Specifies whether or not a specific molecule(s) is/are targeted for
-detection/measurement by the assay ("Yes" or "No"). The CODEX analyte is
-protein.</t>
+        <t>(Required) Indicates whether a specific molecule or set of molecules is targeted
+for detection or measurement by the assay. Example: Yes</t>
       </text>
     </comment>
     <comment ref="G1" authorId="1">
       <text>
-        <t>(Required) An acquisition instrument is the device that contains the signal
-detection hardware and signal processing software. Assays generate signals such
-as light of various intensities or color or signals representing the molecular
-mass.</t>
+        <t>(Required) The company that manufactures or supplies the acquisition instrument.
+An acquisition instrument is a device equipped with signal detection hardware
+and signal processing software. It captures signals produced by assays, such as
+variations in light intensity or color, or signals corresponding to molecular
+mass. If the instrument was custom-built or developed internally, enter
+"In-House". Example: Illumina</t>
       </text>
     </comment>
     <comment ref="H1" authorId="1">
       <text>
-        <t>(Required) Manufacturers of an acquisition instrument may offer various versions
-(models) of that instrument with different features or sensitivities.
-Differences in features or sensitivities may be relevant to processing or
-interpretation of the data.</t>
+        <t>(Required) The specific model of the acquisition instrument, as manufacturers
+often offer various versions with differing features or sensitivities. These
+differences may be relevant to the processing or interpretation of the data. If
+the instrument was custom-built or developed internally, enter "In-House". If
+the model is unknown, enter "Unknown". Example: HiSeq 4000</t>
       </text>
     </comment>
     <comment ref="I1" authorId="1">
       <text>
-        <t>(Required) How long was the source material stored, prior to this sample being
-processed? For assays applied to tissue sections, this would be how long the
-tissue section (e.g., slide) was stored, prior to the assay beginning (e.g.,
-imaging). For assays applied to suspensions such as sequencing, this would be
-how long the suspension was stored before library construction began.</t>
+        <t>(Required) The length of time the sample was stored prior to processing it. For
+assays performed on tissue sections, this refers to how long the tissue section
+(e.g., slide) was stored before the assay began (e.g., imaging). For assays
+performed on suspensions, such as sequencing, it refers to how long the
+suspension was stored before library construction started. Example: 12</t>
       </text>
     </comment>
     <comment ref="J1" authorId="1">
       <text>
-        <t>(Required) The time duration unit of measurement</t>
+        <t>(Required) The unit of measurement used to specify the source storage duration
+value. Example: hour</t>
       </text>
     </comment>
     <comment ref="K1" authorId="1">
       <text>
-        <t>The amount of time since the acquisition instrument was last serviced or
-calibrated. This provides a metric for assessing drift in data capture.</t>
+        <t>The length of time since the acquisition instrument was last serviced or
+calibrated. This provides a metric for assessing drift in data capture. Example:
+10</t>
       </text>
     </comment>
     <comment ref="L1" authorId="1">
       <text>
-        <t>The time unit of measurement</t>
+        <t>The unit of measurement used to specify the time since acquisition instrument
+calibration value. Example: month</t>
       </text>
     </comment>
     <comment ref="M1" authorId="1">
       <text>
-        <t>(Required) The path to the file with the ORCID IDs for all contributors of this
-dataset (e.g., "./extras/contributors.tsv" or "./contributors.tsv"). This is an
-internal metadata field that is just used for ingest.</t>
+        <t>(Required) The name of the file containing the ORCID IDs for all contributors to
+this dataset. Example: ./contributors.csv</t>
       </text>
     </comment>
     <comment ref="N1" authorId="1">
       <text>
-        <t>(Required) The top level directory containing the raw and/or processed data. For
-a single dataset upload this might be "." where as for a data upload containing
-multiple datasets, this would be the directory name for the respective dataset.
-For instance, if the data is within a directory called "TEST001-RK" use syntax
-"./TEST001-RK" for this field. If there are multiple directory levels, use the
-format "./TEST001-RK/Run1/Pass2" in which "Pass2" is the subdirectory where the
-single dataset's data is stored. This is an internal metadata field that is just
-used for ingest.</t>
+        <t>(Required) The top-level directory containing the raw and/or processed data. For
+a single dataset upload, this might be represented as ".", whereas for a data
+upload containing multiple datasets, this would be the directory name for the
+respective dataset. For example, if the data is within a directory named
+"TEST001-RK", use the syntax "./TEST001-RK" for this field. If there are
+multiple directory levels, use the format "./TEST001-RK/Run1/Pass2", where
+"Pass2" is the subdirectory where the single dataset's data is stored. This is
+an internal metadata field used solely for data ingestion. Example: ./TEST001-RK</t>
       </text>
     </comment>
     <comment ref="O1" authorId="1">
       <text>
-        <t>For Visium, this is the area of spots that was covered by tissue within the
-captured area, not the total possible captured area which is fixed. For GeoMx
-this would be the area of the AOI being captured. For HiFi this is the summed
-area of the ROIs in a single flowcell lane. For CosMx and Resolve, this is the
-area of the FOV (aka ROI) region being captured. For Xenium this is the total
-area of the FOV regions (aka ROI) being captured. For Stereo-Seq this is the
-number of beads.</t>
+        <t>The mapped area value, which refers to the specific area covered or captured in
+various assays. For Visium, it is the area of spots covered by tissue within the
+captured area, excluding the total possible captured area. For GeoMx, it refers
+to the area of the AOI being captured. In HiFi, it is the summed area of the
+ROIs in a single flowcell lane. For CosMx and Resolve, it indicates the area of
+the FOV (also known as ROI) region being captured. For Xenium, it is the total
+area of the FOV regions (also known as ROI) being captured. For Stereo-Seq, this
+value represents the number of beads. Example: 42.25</t>
       </text>
     </comment>
     <comment ref="P1" authorId="1">
       <text>
-        <t>The unit of measurement for the mapping area. For Visium and GeoMx this is
-typically um^2.</t>
+        <t>The unit of measurement for the mapped area value. If mapping area is not
+specified, this field may be left blank. Example: um^2</t>
       </text>
     </comment>
     <comment ref="Q1" authorId="1">
       <text>
-        <t>(Required) A unique ID denoting the slide used. This allows users the ability to
+        <t>(Required) The unique identifier assigned to each slide, enabling users to
 determine which tissue sections were processed together on the same slide. It is
-recommended that data providers prefix the ID with the center name, to prevent
-values overlapping across centers.</t>
+recommended that data providers prefix the ID with the center name to prevent
+overlapping values across different centers. Example: VAN0071-PA-1-1_AF</t>
       </text>
     </comment>
     <comment ref="R1" authorId="1">
       <text>
-        <t>Will normally be 100 degrees Celsius for RNA assays, and 80 degrees Celsius for
-protein assays.</t>
+        <t>The incubation temperature required for target retrieval, which is typically 100
+degrees Celsius for RNA assays and 80 degrees Celsius for protein assays.
+Example: 100</t>
       </text>
     </comment>
     <comment ref="S1" authorId="1">
       <text>
-        <t>The duration for which a sample is exposed to a target retrieval solution.</t>
+        <t>The duration for which a sample is exposed to a target retrieval solution.
+Example: 15</t>
       </text>
     </comment>
     <comment ref="T1" authorId="1">
       <text>
-        <t>The units for target retrieval incubation time value.</t>
+        <t>The unit of measurement for the target retrieval incubation time value. If no
+incubation time is specified, this field may be left blank. Example: minute</t>
       </text>
     </comment>
     <comment ref="U1" authorId="1">
       <text>
-        <t>How long was the oligo-conjugated RNA or oligo-conjugated antibody probes
-hybridized with the sample?</t>
+        <t>The duration for which the oligo-conjugated RNA or oligo-conjugated antibody
+probes were hybridized with the sample. Example: 30</t>
       </text>
     </comment>
     <comment ref="V1" authorId="1">
       <text>
-        <t>The units for probe hybridization time value.</t>
+        <t>The unit of measurement for the probe hybridization time value. If the
+hybridization time is not specified, this field may be left blank. Example:
+minute</t>
       </text>
     </comment>
     <comment ref="W1" authorId="1">
       <text>
-        <t>This is the probe panel used to target genes and/or proteins. In cases where
-there is a core panel and add-on modules, the core panel should be selected
-here. If additional panels are used, then they must be included in the
-"additional_panels_used.csv" file that's uploaded with the dataset.</t>
+        <t>The oligo probe panel used to target genes and/or proteins. If there is a core
+panel along with add-on modules, the core panel should be selected in this
+field. Any additional panels utilized should be documented in the
+"additional_panels_used.csv" file, which must be uploaded alongside the dataset.
+Example: 10x Genomics; Visium Human Transcriptome Probe Kit-Small; PN 1000363</t>
       </text>
     </comment>
     <comment ref="X1" authorId="1">
       <text>
-        <t>(Required) State ("Yes" or "No") whether custom RNA or antibody probes were
-used. If custom probes were used, they must be listed in the
-"custom_probe_set.csv" file.</t>
+        <t>(Required) Indicates whether custom RNA or antibody probes were utilized in the
+assay. If custom probes were employed, they should be documented in the
+"custom_probe_set.csv" file. Example: No</t>
       </text>
     </comment>
     <comment ref="Y1" authorId="1">
       <text>
-        <t>(Required) How many genes, RNA isoforms or RNA regions are targeted by probes.</t>
+        <t>The number of panel targets, which refers to the total count of genes, RNA
+isoforms, or RNA regions that are targeted by probes. Example: 1000</t>
       </text>
     </comment>
     <comment ref="Z1" authorId="1">
       <text>
-        <t>A label for the region of interest. For Resolve and CosMx, this is the field of
-view (FOV) label. For Xenium this is the ID of the region containing the
-analysis. For GeoMx this can be found in the "Initial Dataset" spreadsheet
-(download from within Data Analysis Suite).</t>
+        <t>The label for the region of interest (ROI). For Resolve and CosMx, this
+corresponds to the field of view (FOV) label. In the case of Xenium, it refers
+to the ID of the region containing the analysis. For GeoMx, this information can
+be located in the "Initial Dataset" spreadsheet, which can be downloaded from
+within the Data Analysis Suite. Example: Decidua</t>
       </text>
     </comment>
     <comment ref="AA1" authorId="1">
       <text>
-        <t>The overarching anatomical structure.</t>
+        <t>The label for the overarching anatomical structure. If the anatomical structure
+is not applicable or not specified, this field may be left blank. Example:
+Kidney</t>
       </text>
     </comment>
     <comment ref="AB1" authorId="1">
       <text>
-        <t>The ontology ID for the parent structure. Typically this would be an UBERON ID.</t>
+        <t>The ontology ID associated with the anatomical structure, typically represented
+by an UBERON ID. Example: UBERON:0002113</t>
       </text>
     </comment>
     <comment ref="AC1" authorId="1">
       <text>
-        <t>A semicolon separated list of non-shared files to be included in the dataset.
-The path assumes the files are located in the "TOP/non-global/" directory. For
-example, for the file is
-TOP/non-global/lab_processed/images/1-tissue-boundary.geojson the value of this
-field would be "./lab_processed/images/1-tissue-boundary.geojson". After ingest,
-these files will be copied to the appropriate locations within the respective
-dataset directory tree. This field is used for internal HuBMAP processing.
-Examples for GeoMx and PhenoCycler are provided in the File Locations
-documentation:
-https://docs.google.com/document/d/1n2McSs9geA9Eli4QWQaB3c9R3wo5d5U1Xd57DWQfN5Q/edit#heading=h.1u82i4axggee</t>
+        <t>Specifies a semicolon-separated list of non-global files that are to be included
+in the dataset. The file paths assume that the files are located in the
+"TOP/non-global/" directory. For instance, if the file is located at
+TOP/non-global/lab_processed/images/1-tissue-boundary.geojson, the value for
+this field would be "./lab_processed/images/1-tissue-boundary.geojson". Once
+ingested, these files will be copied to their appropriate locations within the
+respective dataset directory tree. This field is intended for internal HuBMAP
+processing. Examples for GeoMx and PhenoCycler are provided in the File
+Locations documentation:
+https://docs.google.com/document/d/1n2McSs9geA9Eli4QWQaB3c9R3wo5d5U1Xd57DWQfN5Q/edit#heading=h.1u82i4axggee
+Example: ./lab_processed/images/1-tissue-boundary.geojson</t>
       </text>
     </comment>
     <comment ref="AD1" authorId="1">
       <text>
-        <t>(Required) The string that serves as the definitive identifier for the metadata
-schema version and is readily interpretable by computers for data validation and
+        <t>The unique string identifier for the metadata specification version, which is
+easily interpretable by computers for purposes of data validation and
 processing. Example: 22bc762a-5020-419d-b170-24253ed9e8d9</t>
       </text>
     </comment>
@@ -254,7 +270,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="450">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1243,6 +1259,12 @@
     <t>https://identifiers.org/RRID:SCR_027095</t>
   </si>
   <si>
+    <t>Panoramic 150 Digital Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_027467</t>
+  </si>
+  <si>
     <t>Aperio AT2</t>
   </si>
   <si>
@@ -1444,6 +1466,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000455</t>
   </si>
   <si>
+    <t>NanoString Technologies; CosMx Mouse Universal Cell Characterization Panel (RNA, 1000 Plex); PN CMX-M-USCP-1KP-R</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000457</t>
+  </si>
+  <si>
     <t>10x Genomics; Xenium Custom Gene Expression Panel (51-100 genes); PN 1000561</t>
   </si>
   <si>
@@ -1474,18 +1502,18 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000362</t>
   </si>
   <si>
+    <t>NanoString Technologies; CosMx Hs WTX RNA Panel Kit, 2 slides: PN 121500047</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000453</t>
+  </si>
+  <si>
     <t>10x Genomics; Xenium Human Lung Gene Expression Panel; PN 1000601</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000443</t>
   </si>
   <si>
-    <t>NanoString Technologies; CosMx Hs WTX RNA Panel Kit, 2 slides; PN 121500047</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000453</t>
-  </si>
-  <si>
     <t>NanoString Technologies; CosMx Mouse Neuroscience Panel (Protein, 64 Plex); PN CMX-M-Neuro-64P-P</t>
   </si>
   <si>
@@ -1573,9 +1601,6 @@
     <t>metadata_schema_id</t>
   </si>
   <si>
-    <t>971357a5-6491-4149-aa6e-d6f14bc9a048</t>
-  </si>
-  <si>
     <t>schema:title</t>
   </si>
   <si>
@@ -1588,7 +1613,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-09-18T09:02:19-07:00</t>
+    <t>2025-10-07T13:10:12-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1756,78 +1781,75 @@
         <v>199</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>438</v>
+        <v>442</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
         <v>34</v>
-      </c>
-      <c r="AD2" t="s" s="31">
-        <v>439</v>
       </c>
     </row>
   </sheetData>
@@ -1845,7 +1867,7 @@
       <formula1>'acquisition_instrument_vendor'!$A$1:$A$30</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$76</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$77</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1887,7 +1909,7 @@
       <formula1>'probe_hybridization_time_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="W2:W1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'oligo_probe_panel'!$A$1:$A$27</formula1>
+      <formula1>'oligo_probe_panel'!$A$1:$A$28</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="X2:X1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_custom_probes_used'!$A$1:$A$2</formula1>
@@ -1913,10 +1935,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -1934,18 +1956,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -1955,7 +1977,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1963,218 +1985,226 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>385</v>
+        <v>387</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>393</v>
+        <v>395</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>395</v>
+        <v>397</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>401</v>
+        <v>403</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>405</v>
+        <v>407</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>407</v>
+        <v>409</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>415</v>
+        <v>417</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>419</v>
+        <v>421</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>425</v>
+        <v>427</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>429</v>
+        <v>431</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>431</v>
+        <v>433</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>434</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>435</v>
       </c>
     </row>
   </sheetData>
@@ -2221,16 +2251,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>445</v>
+        <v>448</v>
       </c>
     </row>
     <row r="2">
@@ -2238,13 +2268,13 @@
         <v>34</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>446</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -3076,7 +3106,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B76"/>
+  <dimension ref="A1:B77"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3688,6 +3718,14 @@
       </c>
       <c r="B76" t="s" s="0">
         <v>348</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="0">
+        <v>349</v>
+      </c>
+      <c r="B77" t="s" s="0">
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -3705,42 +3743,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -3758,26 +3796,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -3795,18 +3833,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix missing metadata schema id
</commit_message>
<xml_diff>
--- a/cosmx-proteomics/latest/cosmx-proteomics.xlsx
+++ b/cosmx-proteomics/latest/cosmx-proteomics.xlsx
@@ -61,7 +61,7 @@
     </comment>
     <comment ref="D1" authorId="1">
       <text>
-        <t>(Required) The specific type of dataset being produced. Example: RNAseq</t>
+        <t>The specific type of dataset being produced. Example: RNAseq</t>
       </text>
     </comment>
     <comment ref="E1" authorId="1">
@@ -106,8 +106,8 @@
     </comment>
     <comment ref="J1" authorId="1">
       <text>
-        <t>(Required) The unit of measurement used to specify the source storage duration
-value. Example: hour</t>
+        <t>The unit of measurement used to specify the source storage duration value.
+Example: hour</t>
       </text>
     </comment>
     <comment ref="K1" authorId="1">
@@ -270,7 +270,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="451">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -1601,6 +1601,9 @@
     <t>metadata_schema_id</t>
   </si>
   <si>
+    <t>971357a5-6491-4149-aa6e-d6f14bc9a048</t>
+  </si>
+  <si>
     <t>schema:title</t>
   </si>
   <si>
@@ -1613,7 +1616,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-10-07T13:10:12-07:00</t>
+    <t>2025-10-09T10:38:31-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1848,8 +1851,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="D2" t="s" s="5">
-        <v>34</v>
+      <c r="AD2" t="s" s="31">
+        <v>443</v>
       </c>
     </row>
   </sheetData>
@@ -2251,16 +2254,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="2">
@@ -2268,13 +2271,13 @@
         <v>34</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
   </sheetData>

</xml_diff>